<commit_message>
rodando os codigos novamente
</commit_message>
<xml_diff>
--- a/data/sumaricao_categorias.xlsx
+++ b/data/sumaricao_categorias.xlsx
@@ -421,97 +421,97 @@
         </is>
       </c>
       <c r="D2">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E2">
-        <v>364307</v>
+        <v>363519</v>
       </c>
       <c r="F2">
-        <v>53489</v>
+        <v>53344</v>
       </c>
       <c r="G2">
-        <v>6544</v>
+        <v>6503</v>
       </c>
       <c r="H2">
-        <v>3859</v>
+        <v>3851</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>BabuSantana, brunogagliasso, YuriMarcal, brunoformiga, essediafoilouco, iglesbiteriana, thiamparo, HistoriaNoPaint, rodrigocapelo, MussumAlive, cinefilo_K, andrefran, LeviKaique, dominiopop, fabiunascimento, Ticostacruz, taliriapetrone, SimoneEhNois, QuebrandoOTabu, startupdareal, aanonnyma, AfroSailor, lolaescreva, ma_azevedo94, Cauefabiano, joelluiz_adv, franca_rodrigo, ReTintaPreta, danielleonawale, knjcheeks_, gaby17pontes, GabiRAR1, rogercipo, davidmirandario, lgqueiroga, heroinadolixo, gleisi, Savagefiction, Pessoa_Cansada, carolizaaando, Rosy_Oliveiira, danvieirass, jpgadelhaof, jojopancada, soutamires_sp, soutoverso, pestodeboldo, LeonelRadde, levieiraprof, MidiaNINJA, caduadv, FellerMarcelo, MarceloUchoa_, EstreLaaany, TeresaCristina, michelpinho, tiamaoficial, luyarafranco, patriers, iamKalera, jhonpaim15, afrocrente, brasil247, Nailahnv, sigaoflavio, sunamita_nobre, jaoseupimenta, hospicio_brasil, TigerGames, HeslaineVieira, livialaranjeira, Crissy_98_, profsosa13, religiaosincera, marioadolfo, esquerdeando, gdoweber, joaofelipenobre, eueoyoon, _rosaneborges, anunesrocha, MariluPamc, buerolol, souljazzca, realodara, livrosdodrii, jfmathias, afro_hey, vanessasoaresc4, DCM_online, mayrasigwalt, waltermoraes_, lucas_kurz, jaciarabri, LianaCirne, Cris_Barbieri, passarosErosas, brauneoficial, blckklucas, donairene13, geekcom2, letparks, oBrunoRomano, Sucubus, refugefefo, SirLucasMatheus, eurickrodrigues, evandrof, AeroportoD, florapaulita, danibacedo, Daniel07091992, jonasdiandrade, beatxriz, jgprates, afroestima2, ChicaoBulhoes, allisonaw1965, orlandoguerreir, rafhaelnep, observint, JeGiacometInda, OManoRogerio, joaooribeiro26, brunnosarttori, drikbarbosa, Pablo_Peixoto, takemeout, monica_benicio, eenrietti, BrunoCostoli, mota97fm, erahsfeliz, desconstrunutri, ovictorjame, gobletofpjo, eusamantalima, bea_brazx, slc_cavalcante, adalto_edno, Sybylla_, mdmdaiane, 1cesgusto, souarthurlima, FredLAFernandes, guirocha82, ashleymlia, llcncl, bragacamila1</t>
+          <t>BabuSantana, brunogagliasso, YuriMarcal, brunoformiga, essediafoilouco, iglesbiteriana, thiamparo, HistoriaNoPaint, rodrigocapelo, MussumAlive, cinefilo_K, andrefran, LeviKaique, dominiopop, fabiunascimento, Ticostacruz, taliriapetrone, SimoneEhNois, QuebrandoOTabu, startupdareal, aanonnyma, AfroSailor, lolaescreva, ma_azevedo94, Cauefabiano, joelluiz_adv, franca_rodrigo, ReTintaPreta, danielleonawale, knjcheeks_, gaby17pontes, GabiRAR1, rogercipo, davidmirandario, lgqueiroga, heroinadolixo, gleisi, Savagefiction, Pessoa_Cansada, carolizaaando, Rosy_Oliveiira, danvieirass, jpgadelhaof, jojopancada, soutamires_sp, soutoverso, pestodeboldo, LeonelRadde, levieiraprof, MidiaNINJA, caduadv, FellerMarcelo, MarceloUchoa_, EstreLaaany, TeresaCristina, michelpinho, tiamaoficial, luyarafranco, patriers, iamKalera, jhonpaim15, afrocrente, Nailahnv, sigaoflavio, sunamita_nobre, jaoseupimenta, hospicio_brasil, TigerGames, HeslaineVieira, livialaranjeira, Crissy_98_, profsosa13, religiaosincera, marioadolfo, esquerdeando, gdoweber, joaofelipenobre, eueoyoon, _rosaneborges, anunesrocha, MariluPamc, buerolol, souljazzca, realodara, livrosdodrii, jfmathias, afro_hey, vanessasoaresc4, mayrasigwalt, waltermoraes_, lucas_kurz, jaciarabri, LianaCirne, Cris_Barbieri, passarosErosas, brauneoficial, blckklucas, donairene13, geekcom2, oBrunoRomano, Sucubus, refugefefo, SirLucasMatheus, eurickrodrigues, evandrof, AeroportoD, florapaulita, danibacedo, Daniel07091992, jonasdiandrade, beatxriz, jgprates, afroestima2, ChicaoBulhoes, allisonaw1965, orlandoguerreir, rafhaelnep, observint, JeGiacometInda, OManoRogerio, joaooribeiro26, brunnosarttori, drikbarbosa, Pablo_Peixoto, takemeout, monica_benicio, eenrietti, BrunoCostoli, mota97fm, erahsfeliz, desconstrunutri, ovictorjame, gobletofpjo, eusamantalima, bea_brazx, slc_cavalcante, adalto_edno, Sybylla_, mdmdaiane, 1cesgusto, souarthurlima, FredLAFernandes, guirocha82, ashleymlia, llcncl, bragacamila1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>contrario</t>
+          <t>favoravel</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"O trainee magalu promove o racismo"</t>
+          <t>"O trainee magalu é uma ação afirmativa desejável"</t>
         </is>
       </c>
       <c r="D3">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="E3">
-        <v>80821</v>
+        <v>94447</v>
       </c>
       <c r="F3">
-        <v>14366</v>
+        <v>10649</v>
       </c>
       <c r="G3">
-        <v>5676</v>
+        <v>2959</v>
       </c>
       <c r="H3">
-        <v>2004</v>
+        <v>1431</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>carlosjordy, LorenzonItalo, profpaulamarisa, LuizCamargoVlog, spinellirio, depheliolopes, josuenunes, BlackDogBC, Desesquerdizada, Jouberth19, romollerSP, rmotta2, FernandoHoliday, Bolsoneas, RRDECA_, Felippe_Hermes, opropriofaka, dezacrvg, CrisMenshova, AlessandroLoio2, simmer_lara, CanaldoNegaoo, LucianaSV29, PastorLiomar, _charizard100, canalCCore2, WagnerThomazoni, thaispsic, JulioOliSantos2, ericayhwh, Sirlene_Emanuel, jaohff, ribas1960, PPReacaFla2, GauchaLih, NA, fabiomello1010, CaioCarlosibg, erickirios, guilhermedecnop, paulocruzphi, teresinhalopes, gabrielferna_a, Arthurdinizrd, kkgbraga, jesus_filha, VlogdoLisboa, FernandoMessina, doxxxx, viniciussexto, ToniTosti1, _VF20, FredRC, MonicaMachado38, nerdclassico, WolfConservador, ajulysantos, rinaldidigilio, thiagosiqueira5</t>
+          <t>thiamparo, danielagomesphd, slpng_giants_pt, DTangerinoPenal, cynaramenezes, jeff_theblack, LeviKaique, QuebrandoOTabu, AndreaMPacha, Savagefiction, tesoureiros, hudsonbonatto, mariliadf2, dasilvabenedita, RMafei, Neka_BR, Ticostacruz, brunnosarttori, Omardeideais, AdrianaCarranca, luisaciteli, GabrielCBrasil, davicalbez, RafaelValim7, NA, fernandapsol, bolsoregrets, srlm, tiamaoficial, luziel__, Sen_Cristovam, andrefran, andrefatala, chambzrs, edufelipe101, agrdeumsm, SamPancher, heelobrandao, marcogomes, anacarla_abrao, franca_rodrigo, passalanorh, GabineteOcio, pbdjulia, TarcisoRenova, potenciasnegras, TatiNefertari, oviniporto, desisalg, isantanax, wendy_andrade, barretonessa, albertocalmeida, andersonsenaxxp, jennieyees, AliQuintiliano, emirsader, jojopancada, rogercipo, Bebeto_Esposito, felip0c, JaumGodoy, Sonia_Cout_, Joao_Gini, lapena, Iberedias, dz7king, mailsonmcj, gamerpobre12344, FamosoLucas_, jgprates, AndreGomesF, luclsluiz, Legurbano, joelluiz_adv, antonionetopdt, EuSouLivres, buruaca, RicardoWeber, teeaggo, naty_andradde, gabrielzep, juliamolusco7, omgerva, kauancoellho, medoedeliriobr, tainadepaularj, SawaraKali, Flavio_Sampaio, _nelsoncezar, Tiagoonie, cruz_elianalves, nathali20044244, ago_almeida, profaflavia, talitismo, hilde_angel</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>outros</t>
+          <t>contrario</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"Matérias jornalísticas"</t>
+          <t>"O trainee magalu promove o racismo"</t>
         </is>
       </c>
       <c r="D4">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="E4">
-        <v>32644</v>
+        <v>80522</v>
       </c>
       <c r="F4">
-        <v>3234</v>
+        <v>14414</v>
       </c>
       <c r="G4">
-        <v>4066</v>
+        <v>5736</v>
       </c>
       <c r="H4">
-        <v>1302</v>
+        <v>2012</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>folha, JornalOGlobo, conexaopolitica, revistaforum, jornalextra, JornalDaCidadeO, Estadao, BlogdoNoblat, UOLNoticias, revistaoeste, congressoemfoco, DiarioPE, UOL, DCM_online, Metropoles, gazetadopovo, CNNBrBusiness, bbcbrasil, exame, elpais_brasil, jc_pe, correio, laurojardim, brasil247, em_com, flaviaol</t>
+          <t>carlosjordy, LorenzonItalo, profpaulamarisa, LuizCamargoVlog, spinellirio, depheliolopes, josuenunes, BlackDogBC, Desesquerdizada, Jouberth19, romollerSP, rmotta2, FernandoHoliday, Bolsoneas, RRDECA_, opropriofaka, dezacrvg, CrisMenshova, AlessandroLoio2, simmer_lara, CanaldoNegaoo, LucianaSV29, PastorLiomar, _charizard100, canalCCore2, WagnerThomazoni, thaispsic, JulioOliSantos2, ericayhwh, Sirlene_Emanuel, jaohff, ribas1960, PPReacaFla2, GauchaLih, NA, fabiomello1010, CaioCarlosibg, erickirios, guilhermedecnop, paulocruzphi, teresinhalopes, gabrielferna_a, Arthurdinizrd, kkgbraga, jesus_filha, VlogdoLisboa, FernandoMessina, doxxxx, viniciussexto, ToniTosti1, _VF20, FredRC, MonicaMachado38, nerdclassico, WolfConservador, ajulysantos, rinaldidigilio, thiagosiqueira5</t>
         </is>
       </c>
     </row>
@@ -523,69 +523,69 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>98</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"Posicionamento não identificado"</t>
+          <t>"Matérias jornalísticas"</t>
         </is>
       </c>
       <c r="D5">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E5">
-        <v>23301</v>
+        <v>39630</v>
       </c>
       <c r="F5">
-        <v>2127</v>
+        <v>4327</v>
       </c>
       <c r="G5">
-        <v>1043</v>
+        <v>4407</v>
       </c>
       <c r="H5">
-        <v>664</v>
+        <v>1601</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>LorenzonItalo, JoaquinTeixeira, andrezadelgado, alfapobre, Dudu, rmotta2, eugleidistone, jpgadelhaof, canaldasbee, LeticiaShirakin, jlbraga, luide, MussumAlive, jr_mau, paulocruzphi, ittsquel, alisc, GirassolRafa, nathali20044244, sensoinc, FredRC, dedehcamargo, Savagefiction, tesoureiros, FitcherNick, f_alperowitch, brunanarcizo, femisapien_z, ChampMargareth, luccaoneal, TarcisoRenova, JuanSavedra_, souarthurlima, _giovanirocha, artedaguerracnl, IzaVicent, canalCCore2, dannielduque, tucainadobrasil, pensandoaltorc, JacyCarvalho, raythetrouxa, nouvelian, Rayctjay, DanoBessa, Lethiscya, reclamiranda, madeleinelacsko, FriedHardt, DanielQuinzel, wasabinoolho, medoedeliriobr, joaolordelo, sarahemmyli, rdfmedeiros, claudferraz, afroestima2, biraiorio</t>
+          <t>folha, exame, JornalOGlobo, conexaopolitica, revistaforum, jornalextra, brasil247, JornalDaCidadeO, Estadao, BlogdoNoblat, UOLNoticias, revistaoeste, congressoemfoco, DiarioPE, UOL, DCM_online, Metropoles, gazetadopovo, CNNBrBusiness, bbcbrasil, elpais_brasil, jc_pe, madeleinelacsko, correio, laurojardim, em_com, flaviaol</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>contrario</t>
+          <t>outros</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>99</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"Posicionamentos contrários variados"</t>
+          <t>"Posicionamento não identificado"</t>
         </is>
       </c>
       <c r="D6">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E6">
-        <v>21561</v>
+        <v>11416</v>
       </c>
       <c r="F6">
-        <v>1755</v>
+        <v>840</v>
       </c>
       <c r="G6">
-        <v>624</v>
+        <v>568</v>
       </c>
       <c r="H6">
-        <v>379</v>
+        <v>498</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>thiamparo, hoc111, paulocruzphi, AdrianaCarranca, CrysthianeA, thaispsic, mattlimn, gramich, jojopancada, marcogomes, sourodrii, m_blazar, _Renato, EKrominski, TchiMad, de_botequim</t>
+          <t>andrezadelgado, jpgadelhaof, canaldasbee, luide, MussumAlive, paulocruzphi, ittsquel, alisc, GirassolRafa, nathali20044244, FredRC, dedehcamargo, Savagefiction, tesoureiros, brunanarcizo, femisapien_z, ChampMargareth, luccaoneal, TarcisoRenova, JuanSavedra_, souarthurlima, _giovanirocha, artedaguerracnl, IzaVicent, sourodrii, dannielduque, JacyCarvalho, Rayctjay, Lethiscya, reclamiranda, wasabinoolho, joaolordelo, rdfmedeiros, afroestima2, biraiorio</t>
         </is>
       </c>
     </row>
@@ -634,32 +634,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"O trainee magalu realiza um 'apartheid' na sociedade"</t>
+          <t>"Posicionamentos contrários variados"</t>
         </is>
       </c>
       <c r="D8">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E8">
-        <v>3706</v>
+        <v>8008</v>
       </c>
       <c r="F8">
-        <v>596</v>
+        <v>998</v>
       </c>
       <c r="G8">
-        <v>291</v>
+        <v>510</v>
       </c>
       <c r="H8">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>nerdclassico, carlinhoscury, LucianaSV29, SantoElayne2020, Nivea_SpesEst, carlaguimaraes7, CRCF_84, MarizMarcella, mjmacul_lima, paulocnf, fernando_g_f_</t>
+          <t>hoc111, paulocruzphi, rmotta2, Felippe_Hermes, CrysthianeA, thaispsic, mattlimn, gramich, canalCCore2, m_blazar, _Renato, EKrominski, TchiMad, de_botequim</t>
         </is>
       </c>
     </row>
@@ -671,57 +671,69 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"Aceitação apenas de critérios universais"</t>
+          <t>"O trainee magalu realiza um 'apartheid' na sociedade"</t>
         </is>
       </c>
       <c r="D9">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E9">
-        <v>3316</v>
+        <v>3706</v>
       </c>
       <c r="F9">
-        <v>465</v>
+        <v>596</v>
       </c>
       <c r="G9">
-        <v>151</v>
+        <v>291</v>
       </c>
       <c r="H9">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>nerdclassico, lpdossj, LucianaSV29, letparks, sampaio19091, julioreis78, Alpargatas11, Buzz91272883, moneymakerbr</t>
+          <t>nerdclassico, carlinhoscury, LucianaSV29, SantoElayne2020, Nivea_SpesEst, carlaguimaraes7, CRCF_84, MarizMarcella, mjmacul_lima, paulocnf, fernando_g_f_</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>favoravel</t>
+          <t>contrario</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"O trainee magalu é uma ação afirmativa desejável"</t>
+          <t>"Aceitação apenas de critérios universais"</t>
         </is>
       </c>
       <c r="D10">
-        <v>109</v>
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>3504</v>
+      </c>
+      <c r="F10">
+        <v>476</v>
+      </c>
+      <c r="G10">
+        <v>152</v>
+      </c>
+      <c r="H10">
+        <v>39</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>danielagomesphd, slpng_giants_pt, exame, DTangerinoPenal, cynaramenezes, jeff_theblack, LeviKaique, QuebrandoOTabu, AndreaMPacha, Savagefiction, tesoureiros, hudsonbonatto, mariliadf2, dasilvabenedita, RMafei, Neka_BR, Ticostacruz, brunnosarttori, Omardeideais, luisaciteli, GabrielCBrasil, brasil247, davicalbez, RafaelValim7, NA, thiamparo, fernandapsol, bolsoregrets, srlm, tiamaoficial, luziel__, Sen_Cristovam, andrefran, andrefatala, chambzrs, edufelipe101, depheliolopes, agrdeumsm, SamPancher, heelobrandao, marcogomes, anacarla_abrao, franca_rodrigo, passalanorh, GabineteOcio, pbdjulia, TarcisoRenova, potenciasnegras, TatiNefertari, oviniporto, desisalg, isantanax, wendy_andrade, barretonessa, albertocalmeida, andersonsenaxxp, jennieyees, AliQuintiliano, emirsader, rogercipo, Bebeto_Esposito, felip0c, JaumGodoy, Sonia_Cout_, Joao_Gini, lapena, Felippe_Hermes, Iberedias, dz7king, mailsonmcj, gamerpobre12344, FamosoLucas_, jgprates, AndreGomesF, luclsluiz, Legurbano, joelluiz_adv, antonionetopdt, EuSouLivres, buruaca, RicardoWeber, teeaggo, naty_andradde, gabrielzep, juliamolusco7, omgerva, kauancoellho, tainadepaularj, SawaraKali, Flavio_Sampaio, _nelsoncezar, Tiagoonie, cruz_elianalves, nathali20044244, ago_almeida, profaflavia, talitismo, hilde_angel</t>
+          <t>nerdclassico, lpdossj, LucianaSV29, letparks, sampaio19091, julioreis78, Alpargatas11, Buzz91272883, moneymakerbr</t>
         </is>
       </c>
     </row>

</xml_diff>